<commit_message>
Commit solucion errores dependencias samuel
</commit_message>
<xml_diff>
--- a/samuel/fear2.xlsx
+++ b/samuel/fear2.xlsx
@@ -424,10 +424,10 @@
         <v>2.2233125</v>
       </c>
       <c r="E2">
-        <v>-0.7999373551860802</v>
+        <v>-0.7999373551860809</v>
       </c>
       <c r="F2">
-        <v>0.1501104971070012</v>
+        <v>0.1501104971070016</v>
       </c>
       <c r="G2">
         <v>0</v>

</xml_diff>